<commit_message>
jump navbar + window on exe
</commit_message>
<xml_diff>
--- a/information.xlsx
+++ b/information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lluis\Desktop\Projects\automatic_personal_page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4B5D22-2419-4373-AB6A-B56A54EDB6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF6B04E-65E5-4FE1-ACD2-68BC5CCEE912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{9CEA0154-E674-4F6E-9626-759C59FC0DAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="1" activeTab="6" xr2:uid="{9CEA0154-E674-4F6E-9626-759C59FC0DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="ABOUT" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,9 @@
     <sheet name="COURSES" sheetId="5" r:id="rId4"/>
     <sheet name="SKILLS" sheetId="6" r:id="rId5"/>
     <sheet name="PROJECTS" sheetId="2" r:id="rId6"/>
-    <sheet name="EXTRA_INFO" sheetId="10" r:id="rId7"/>
-    <sheet name="LANGUAGES" sheetId="7" r:id="rId8"/>
-    <sheet name="OTHER_INFO" sheetId="8" r:id="rId9"/>
-    <sheet name="CONTACT" sheetId="9" r:id="rId10"/>
+    <sheet name="OTHER" sheetId="8" r:id="rId7"/>
+    <sheet name="CONTACT" sheetId="9" r:id="rId8"/>
+    <sheet name="CUSTOM" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="119">
   <si>
     <t>NAME</t>
   </si>
@@ -833,7 +832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{065832F7-8460-4346-95F7-2D7BFBE41741}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -902,44 +901,6 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00880507-045B-41B2-9D0D-884517C5BB18}"/>
     <hyperlink ref="H2" r:id="rId2" xr:uid="{7070BC93-5CEE-4700-AA56-2B13CDA4802C}"/>
     <hyperlink ref="G2" r:id="rId3" xr:uid="{F500704E-4F43-401A-88CC-5270C1A2ACB4}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8CA0F9-1E61-4B6E-A4DD-4A89ECA2E29E}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="65.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{642C64C2-E5C8-4EE6-B82D-A0D0358E8E35}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1419,6 +1380,110 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BCBF17-B846-480B-A437-F9769858B36E}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8CA0F9-1E61-4B6E-A4DD-4A89ECA2E29E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="65.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{642C64C2-E5C8-4EE6-B82D-A0D0358E8E35}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37FAC5C-5DFF-412F-A2E6-43E8334D15FC}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -1612,80 +1677,4 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA618CF-91CC-4817-A466-B6D90C9FF72A}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BCBF17-B846-480B-A437-F9769858B36E}">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>